<commit_message>
NUEVO FORMATO DE COMPARATIVO
</commit_message>
<xml_diff>
--- a/Sistemas/CCFN-D002-A13-R00 Formato de verificación de basculas.xlsx
+++ b/Sistemas/CCFN-D002-A13-R00 Formato de verificación de basculas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SISTEMAS\Documents\CLAUDIA\PROYECTOS\DOCUMENTACION PROYECTOS\D-FORMATOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT\Documents\GitHub\Formatos\Sistemas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -452,6 +452,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -478,18 +490,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -700,11 +700,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Etiquetadora</a:t>
@@ -783,11 +784,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Recibo</a:t>
@@ -866,11 +868,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Punto de Venta</a:t>
@@ -949,11 +952,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Plataforma</a:t>
@@ -1032,11 +1036,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Satisfactoria</a:t>
@@ -1115,11 +1120,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Regular</a:t>
@@ -1198,11 +1204,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Insatisfactoria</a:t>
@@ -1281,11 +1288,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Satisfactoria</a:t>
@@ -1364,11 +1372,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Regular</a:t>
@@ -1447,11 +1456,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Insatisfactoria</a:t>
@@ -1530,11 +1540,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Satisfactoria</a:t>
@@ -1613,11 +1624,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Regular</a:t>
@@ -1696,11 +1708,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Insatisfactoria</a:t>
@@ -1779,11 +1792,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>No Aplica</a:t>
@@ -1862,11 +1876,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Satisfactoria</a:t>
@@ -1945,11 +1960,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Regular</a:t>
@@ -2028,11 +2044,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Insatisfactoria</a:t>
@@ -2111,11 +2128,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Satisfactoria</a:t>
@@ -2194,11 +2212,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Regular</a:t>
@@ -2277,11 +2296,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Insatisfactoria</a:t>
@@ -2360,11 +2380,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Satisfactoria</a:t>
@@ -2443,11 +2464,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Regular</a:t>
@@ -2526,11 +2548,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Insatisfactoria</a:t>
@@ -2609,11 +2632,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>No Aplica</a:t>
@@ -2692,11 +2716,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>No Aplica</a:t>
@@ -2775,11 +2800,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Satisfactoria</a:t>
@@ -2858,11 +2884,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Regular</a:t>
@@ -2941,11 +2968,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Insatisfactoria</a:t>
@@ -3024,11 +3052,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Satisfactoria</a:t>
@@ -3107,11 +3136,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Regular</a:t>
@@ -3190,11 +3220,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="es-MX" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
+                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Insatisfactoria</a:t>
@@ -3561,10 +3592,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B3:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3577,36 +3611,36 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="18"/>
-      <c r="C3" s="17" t="s">
+      <c r="B3" s="22"/>
+      <c r="C3" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="22" t="s">
+      <c r="D3" s="21"/>
+      <c r="E3" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="19"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="18"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="24" t="s">
+      <c r="B4" s="22"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="20"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="24"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="18"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="24" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="25"/>
-      <c r="G5" s="21"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="25"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
@@ -3629,14 +3663,14 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
@@ -3691,14 +3725,14 @@
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
@@ -3783,14 +3817,14 @@
       <c r="G24" s="10"/>
     </row>
     <row r="25" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
@@ -3923,14 +3957,14 @@
       <c r="G40" s="10"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="26" t="s">
+      <c r="B41" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="26"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
@@ -4011,35 +4045,35 @@
       <c r="G50" s="2"/>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="29" t="s">
+      <c r="B51" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C51" s="29"/>
+      <c r="C51" s="20"/>
       <c r="D51" s="2"/>
-      <c r="E51" s="29" t="s">
+      <c r="E51" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F51" s="29"/>
-      <c r="G51" s="29"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
     <mergeCell ref="B41:G41"/>
     <mergeCell ref="B25:G25"/>
     <mergeCell ref="B15:G15"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="E51:G51"/>
     <mergeCell ref="B51:C51"/>
-    <mergeCell ref="C3:D5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="97" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">

</xml_diff>